<commit_message>
add hyperlinks to all sheets
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/tabs.xlsx
+++ b/src/main/webapp/WEB-INF/books/tabs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/tutorial/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B60117B-6D78-BE4D-9628-BB0D2CCBDE2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A789D8C-A260-BD4A-929A-F69A169F0E5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36780" yWindow="1460" windowWidth="28040" windowHeight="17440" xr2:uid="{8510FC66-29CD-0942-AA25-9D84277BE69E}"/>
+    <workbookView xWindow="2480" yWindow="1940" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{8510FC66-29CD-0942-AA25-9D84277BE69E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cable TV" sheetId="3" r:id="rId1"/>
@@ -29,12 +29,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Cable TV</t>
   </si>
   <si>
     <t>Spectrum</t>
+  </si>
+  <si>
+    <t>child1</t>
+  </si>
+  <si>
+    <t>child2</t>
   </si>
 </sst>
 </file>
@@ -399,7 +405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{697461DE-D753-064A-9400-50E62D70B4C7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -417,10 +423,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0863B39-9A97-2241-B075-4C7825FE079F}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,10 +441,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="'Cable TV'!A1" display="Cable TV" xr:uid="{62BEC13C-F1C1-1248-981F-4237E53D97F2}"/>
     <hyperlink ref="A2" location="Spectrum!A1" display="Spectrum" xr:uid="{18EA6A3D-F283-BF4D-986C-4155431A2707}"/>
+    <hyperlink ref="A3" location="child1!A1" display="child1" xr:uid="{1558ED65-2532-8849-A5B5-3D2D9AD25198}"/>
+    <hyperlink ref="A4" location="child2!A1" display="child2" xr:uid="{21BF6EA7-7668-784C-BD6A-DBD364336E7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update according to use case
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/tabs.xlsx
+++ b/src/main/webapp/WEB-INF/books/tabs.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/tutorial/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A789D8C-A260-BD4A-929A-F69A169F0E5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AB3520-FD8C-F544-A83C-6DBE0AB91944}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2480" yWindow="1940" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{8510FC66-29CD-0942-AA25-9D84277BE69E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cable TV" sheetId="3" r:id="rId1"/>
-    <sheet name="Index" sheetId="2" r:id="rId2"/>
-    <sheet name="Spectrum" sheetId="1" r:id="rId3"/>
-    <sheet name="child1" sheetId="4" r:id="rId4"/>
-    <sheet name="child2" sheetId="5" r:id="rId5"/>
+    <sheet name="Index" sheetId="2" r:id="rId1"/>
+    <sheet name="Cable TV" sheetId="3" r:id="rId2"/>
+    <sheet name="parentA" sheetId="1" r:id="rId3"/>
+    <sheet name="parentB" sheetId="6" r:id="rId4"/>
+    <sheet name="b-1" sheetId="7" state="hidden" r:id="rId5"/>
+    <sheet name="b-2" sheetId="8" state="hidden" r:id="rId6"/>
+    <sheet name="a-1" sheetId="4" state="hidden" r:id="rId7"/>
+    <sheet name="a-2" sheetId="5" state="hidden" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,18 +32,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Cable TV</t>
   </si>
   <si>
-    <t>Spectrum</t>
-  </si>
-  <si>
-    <t>child1</t>
-  </si>
-  <si>
-    <t>child2</t>
+    <t>a-1</t>
+  </si>
+  <si>
+    <t>a-2</t>
+  </si>
+  <si>
+    <t>parentA</t>
+  </si>
+  <si>
+    <t>parentB</t>
+  </si>
+  <si>
+    <t>b-1</t>
+  </si>
+  <si>
+    <t>b-2</t>
   </si>
 </sst>
 </file>
@@ -402,11 +414,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0863B39-9A97-2241-B075-4C7825FE079F}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Cable TV'!A1" display="Cable TV" xr:uid="{62BEC13C-F1C1-1248-981F-4237E53D97F2}"/>
+    <hyperlink ref="A2" location="parentA!A1" display="parentA" xr:uid="{18EA6A3D-F283-BF4D-986C-4155431A2707}"/>
+    <hyperlink ref="A3" location="'a-1'!A1" display="a-1" xr:uid="{1558ED65-2532-8849-A5B5-3D2D9AD25198}"/>
+    <hyperlink ref="A4" location="Index!A1" display="a-2" xr:uid="{21BF6EA7-7668-784C-BD6A-DBD364336E7C}"/>
+    <hyperlink ref="A5" location="Index!A1" display="parentB" xr:uid="{55133DCC-0F46-2648-A67C-9C1DEEA5AB8A}"/>
+    <hyperlink ref="A6" location="Index!A1" display="b-1" xr:uid="{3B76C44E-88A4-B444-94A5-CE7CF74CA67F}"/>
+    <hyperlink ref="A7" location="Index!A1" display="b-2" xr:uid="{EE9B4C4D-1B7A-A84E-832B-95DEC51D81AB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{697461DE-D753-064A-9400-50E62D70B4C7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -421,58 +492,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0863B39-9A97-2241-B075-4C7825FE079F}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Cable TV'!A1" display="Cable TV" xr:uid="{62BEC13C-F1C1-1248-981F-4237E53D97F2}"/>
-    <hyperlink ref="A2" location="Spectrum!A1" display="Spectrum" xr:uid="{18EA6A3D-F283-BF4D-986C-4155431A2707}"/>
-    <hyperlink ref="A3" location="child1!A1" display="child1" xr:uid="{1558ED65-2532-8849-A5B5-3D2D9AD25198}"/>
-    <hyperlink ref="A4" location="child2!A1" display="child2" xr:uid="{21BF6EA7-7668-784C-BD6A-DBD364336E7C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C50F57-ED0D-A94D-84C4-440A81D7A089}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -481,6 +516,59 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B96ADD3-85A3-C342-84B4-AD4905FA7F8F}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9163725-E3A4-B442-9F4B-17A1353EF5CD}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1632780-D935-994A-B309-885C20D48A53}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47F02A1-8A04-3241-8FD5-EB49FDDF8B63}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -495,7 +583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B08002-3257-4143-9670-F07E5AE8CC11}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>

</xml_diff>